<commit_message>
4 Year v2 Time Table Released.
</commit_message>
<xml_diff>
--- a/Time-Table-2023-24/Lab-details/Lab Requirements for 2023-2024 CSD Report.xlsx
+++ b/Time-Table-2023-24/Lab-details/Lab Requirements for 2023-2024 CSD Report.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HEMANTH\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AY-2022-23\Time-Table-2022-23\Time-Table-2023-24\Lab-details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DFF580-F1A1-4273-AE20-CBFF303CD746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="8880" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17194" windowHeight="5384"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Requirements" sheetId="1" r:id="rId1"/>
@@ -234,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,23 +618,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -671,23 +653,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -863,26 +828,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.296875" customWidth="1"/>
+    <col min="3" max="3" width="41.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.09765625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="24" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.296875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
@@ -898,7 +863,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
@@ -914,7 +879,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
@@ -930,7 +895,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>62</v>
       </c>
@@ -942,7 +907,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -968,7 +933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="69.849999999999994" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -994,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>63</v>
       </c>
@@ -1006,7 +971,7 @@
       <c r="G9" s="24"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="69.849999999999994" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1056,7 +1021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>61</v>
       </c>
@@ -1068,7 +1033,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -1118,7 +1083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="20.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -1144,7 +1109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -1168,7 +1133,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>60</v>
       </c>
@@ -1180,7 +1145,7 @@
       <c r="G21" s="24"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -1230,7 +1195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -1250,7 +1215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>3</v>
       </c>
@@ -1276,7 +1241,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>59</v>
       </c>
@@ -1288,7 +1253,7 @@
       <c r="G28" s="24"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1334,7 +1299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1354,7 +1319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>58</v>
       </c>
@@ -1366,7 +1331,7 @@
       <c r="G34" s="24"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>0</v>
       </c>
@@ -1390,7 +1355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="41.95" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>1</v>
       </c>
@@ -1414,7 +1379,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -1436,7 +1401,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>3</v>
       </c>
@@ -1471,34 +1436,35 @@
     <mergeCell ref="A14:G14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" display="http://www.codeblocks.org/downloads/26" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F11" r:id="rId5" display="http://www.codeblocks.org/downloads/26" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F25" r:id="rId6" location="download" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F6" r:id="rId1" display="http://www.codeblocks.org/downloads/26"/>
+    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F23" r:id="rId3"/>
+    <hyperlink ref="F17" r:id="rId4"/>
+    <hyperlink ref="F11" r:id="rId5" display="http://www.codeblocks.org/downloads/26"/>
+    <hyperlink ref="F25" r:id="rId6" location="download"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:G9"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F7" sqref="F7:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.69921875" customWidth="1"/>
+    <col min="7" max="7" width="33.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="6:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:7" ht="14.55" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="6:7" ht="33.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F7" s="14" t="s">
         <v>22</v>
       </c>
@@ -1506,7 +1472,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="6:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:7" ht="20.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F8" s="12" t="s">
         <v>24</v>
       </c>
@@ -1514,7 +1480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="6:7" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:7" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F9" s="13" t="s">
         <v>25</v>
       </c>

</xml_diff>